<commit_message>
fix: Update ultimas respostas
</commit_message>
<xml_diff>
--- a/form.xlsx
+++ b/form.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Limpeza dos dados" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="142">
   <si>
     <t xml:space="preserve">Carimbo de data/hora</t>
   </si>
@@ -176,7 +176,7 @@
     <t xml:space="preserve">Desenvolvedor - Backend</t>
   </si>
   <si>
-    <t xml:space="preserve">Marketing, Vendas</t>
+    <t xml:space="preserve">Marketing</t>
   </si>
   <si>
     <t xml:space="preserve">Automação de builds, Monitoramento e logging, Colaboração e comunicação</t>
@@ -191,19 +191,16 @@
     <t xml:space="preserve">O óbvio seria a automação de processos de testes e deploy. Mas, na minha opinião, o maior benefício é o próprio estímulo e formalização de hábitos de desenvolvimento mais saudáveis, dentre eles a criação de testes para validar funcionalidades e a normalização do tamanho e propósito de cada commit.</t>
   </si>
   <si>
-    <t xml:space="preserve">Marketing</t>
-  </si>
-  <si>
     <t xml:space="preserve">Outro</t>
   </si>
   <si>
     <t xml:space="preserve">SVN</t>
   </si>
   <si>
-    <t xml:space="preserve">Transporte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ferramenta própria </t>
+    <t xml:space="preserve">Logistica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ferramenta própria</t>
   </si>
   <si>
     <t xml:space="preserve">Travis CI</t>
@@ -245,7 +242,7 @@
     <t xml:space="preserve">Agilidade em processos </t>
   </si>
   <si>
-    <t xml:space="preserve">Saúde, Social e financeiro</t>
+    <t xml:space="preserve">Saúde</t>
   </si>
   <si>
     <t xml:space="preserve">Nenhuma</t>
@@ -272,9 +269,6 @@
     <t xml:space="preserve">Estagiário</t>
   </si>
   <si>
-    <t xml:space="preserve">Logistica</t>
-  </si>
-  <si>
     <t xml:space="preserve">Azure Devops</t>
   </si>
   <si>
@@ -317,9 +311,6 @@
     <t xml:space="preserve">Govtech</t>
   </si>
   <si>
-    <t xml:space="preserve">Ecommerce, Marketing</t>
-  </si>
-  <si>
     <t xml:space="preserve">Trello, ClickUp</t>
   </si>
   <si>
@@ -339,6 +330,84 @@
   </si>
   <si>
     <t xml:space="preserve">A vantagens de  atuar o processo em desenvolvimento de software,ele permite a controlar as entradas e saídas dos produtos de maneira de automática,com eficiência e segurança.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DevOps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jenkins, GitLab CI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diariamente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvedor Full Stack / Engenheiro de Software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hotel Chatbot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jira, Miro, LucidChart (fluxogramas), Planilhas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testes automatizados, Deploy contínuo, Colaboração e comunicação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O maior desafio é fazer as pessoas, de diferentes níveis, usarem as ferramentas corretamente e seguirem todos os passos durante e após o desenvolvimento, para que o processo possa se tornar uma cultura da empresa. Isso acaba sendo uma desvantagem em certo momento porque pode gerar uma ruptura de ideias nas equipes, e até que vire uma cultura as coisas podem ficar meio bagunçadas ou até mesmo nem todos aceitarem.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A vantagem é a facilitação que as ferramentas trazem, ter testes automatizados, deploy continuo e tasks mapeadas facilita muito na hora de planejar novas sprints e também quando é necessário buscar algum histórico de alguma coisa feita no passado, pois acaba que tudo fica documentado de certa forma nas ferramentas, possibilitando ter toda a linha do tempo de um projeto caso seja necessário. Além disso, com algumas ferramentas e possível levantar estatísticas e gráficos, que podem auxiliar no planejamento ou até mesmo na métrica de resultados.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Financeira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redmine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automação de builds, Deploy contínuo, Colaboração e comunicação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CircleCI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gitea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvedor - Full stack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comércio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Movidesk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bitbucket pipelines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zoho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Não utiliza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definição de prioridades.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Histórico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mais de 50 pessoas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Financeiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ferramenta interna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">segurança no deploy, sem risco de erro humano</t>
   </si>
   <si>
     <t xml:space="preserve">1. Qual função você desempenha no processo de desenvolvimento de software?</t>
@@ -389,7 +458,7 @@
     <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm:ss"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -418,6 +487,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -462,7 +537,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -487,6 +562,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,13 +585,13 @@
   </sheetPr>
   <dimension ref="A1:N128"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="bottomLeft" activeCell="N11" activeCellId="0" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.8125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="61"/>
@@ -852,13 +931,13 @@
         <v>25</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>48</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>37</v>
@@ -890,19 +969,19 @@
         <v>50</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>20</v>
@@ -911,7 +990,7 @@
         <v>2</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K9" s="4" t="n">
         <v>5</v>
@@ -940,7 +1019,7 @@
         <v>43</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>18</v>
@@ -955,7 +1034,7 @@
         <v>2</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K10" s="4" t="n">
         <v>5</v>
@@ -964,10 +1043,10 @@
         <v>39</v>
       </c>
       <c r="M10" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="N10" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -981,7 +1060,7 @@
         <v>15</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>17</v>
@@ -999,7 +1078,7 @@
         <v>3</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K11" s="4" t="n">
         <v>5</v>
@@ -1043,7 +1122,7 @@
         <v>4</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K12" s="4" t="n">
         <v>5</v>
@@ -1087,7 +1166,7 @@
         <v>3</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K13" s="4" t="n">
         <v>5</v>
@@ -1131,7 +1210,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K14" s="4" t="n">
         <v>5</v>
@@ -1166,10 +1245,10 @@
         <v>18</v>
       </c>
       <c r="G15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="I15" s="4" t="n">
         <v>3</v>
@@ -1187,7 +1266,7 @@
         <v>22</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1204,10 +1283,10 @@
         <v>25</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>36</v>
@@ -1219,7 +1298,7 @@
         <v>3</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K16" s="4" t="n">
         <v>5</v>
@@ -1283,7 +1362,7 @@
         <v>45455.6718279745</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>15</v>
@@ -1307,7 +1386,7 @@
         <v>4</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K18" s="4" t="n">
         <v>5</v>
@@ -1327,7 +1406,7 @@
         <v>45455.8141923032</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>15</v>
@@ -1336,10 +1415,10 @@
         <v>25</v>
       </c>
       <c r="E19" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>19</v>
@@ -1357,7 +1436,7 @@
         <v>5</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M19" s="0" t="s">
         <v>22</v>
@@ -1380,13 +1459,13 @@
         <v>43</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>20</v>
@@ -1395,7 +1474,7 @@
         <v>4</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K20" s="4" t="n">
         <v>4</v>
@@ -1415,7 +1494,7 @@
         <v>45456.8268721759</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>15</v>
@@ -1439,7 +1518,7 @@
         <v>4</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K21" s="4" t="n">
         <v>5</v>
@@ -1459,7 +1538,7 @@
         <v>45456.8356572685</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>15</v>
@@ -1471,7 +1550,7 @@
         <v>17</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>19</v>
@@ -1483,7 +1562,7 @@
         <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K22" s="4" t="n">
         <v>5</v>
@@ -1515,7 +1594,7 @@
         <v>17</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>36</v>
@@ -1547,7 +1626,7 @@
         <v>45456.8613598727</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>15</v>
@@ -1556,22 +1635,22 @@
         <v>25</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F24" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="G24" s="4" t="s">
-        <v>91</v>
-      </c>
       <c r="H24" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I24" s="4" t="n">
         <v>3</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K24" s="4" t="n">
         <v>5</v>
@@ -1580,10 +1659,10 @@
         <v>53</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1600,13 +1679,13 @@
         <v>43</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>20</v>
@@ -1615,7 +1694,7 @@
         <v>3</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K25" s="4" t="n">
         <v>5</v>
@@ -1638,28 +1717,28 @@
         <v>14</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I26" s="4" t="n">
         <v>2</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K26" s="4" t="n">
         <v>5</v>
@@ -1688,13 +1767,13 @@
         <v>25</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>98</v>
+        <v>17</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>20</v>
@@ -1703,7 +1782,7 @@
         <v>4</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K27" s="4" t="n">
         <v>5</v>
@@ -1712,10 +1791,10 @@
         <v>53</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1732,13 +1811,13 @@
         <v>25</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>98</v>
+        <v>17</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H28" s="4" t="s">
         <v>20</v>
@@ -1747,7 +1826,7 @@
         <v>4</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K28" s="4" t="n">
         <v>5</v>
@@ -1756,38 +1835,407 @@
         <v>53</v>
       </c>
       <c r="M28" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="n">
+        <v>45460.7829762616</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="N28" s="4" t="s">
+      <c r="H29" s="4" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="2"/>
+      <c r="I29" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K29" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M29" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N29" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="2"/>
+      <c r="A30" s="3" t="n">
+        <v>45461.0021015046</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="K30" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="2"/>
+      <c r="A31" s="3" t="n">
+        <v>45461.6181952431</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I31" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="K31" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="L31" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M31" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N31" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="2"/>
+      <c r="A32" s="3" t="n">
+        <v>45461.6536970139</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K32" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M32" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N32" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="2"/>
+      <c r="A33" s="3" t="n">
+        <v>45461.6565365741</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K33" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M33" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N33" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="2"/>
+      <c r="A34" s="3" t="n">
+        <v>45461.6595517824</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I34" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K34" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M34" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N34" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="2"/>
+      <c r="A35" s="3" t="n">
+        <v>45461.6685216898</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I35" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K35" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M35" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N35" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D36" s="2"/>
+      <c r="A36" s="3" t="n">
+        <v>45461.7605780556</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K36" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="2"/>
+      <c r="A37" s="3" t="n">
+        <v>45461.789567581</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I37" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K37" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M37" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="N37" s="4" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D38" s="2"/>
@@ -2080,78 +2528,78 @@
   </sheetPr>
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="167.74"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>112</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>113</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>